<commit_message>
Add job day to UI for easy selection.
</commit_message>
<xml_diff>
--- a/server/prasignups8-2-2015.xlsx
+++ b/server/prasignups8-2-2015.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="179">
   <si>
     <t>Name</t>
   </si>
@@ -115,9 +115,15 @@
     <t>czd5FSdZhg</t>
   </si>
   <si>
+    <t>Courtney Walker</t>
+  </si>
+  <si>
     <t>Front Gate Help/Start Gate</t>
   </si>
   <si>
+    <t>di6p9JLS0f</t>
+  </si>
+  <si>
     <t>wdevpYXEOR</t>
   </si>
   <si>
@@ -133,9 +139,15 @@
     <t>QHpKgN0UyI</t>
   </si>
   <si>
+    <t>Matt Jones</t>
+  </si>
+  <si>
     <t>Finish Line Flagger</t>
   </si>
   <si>
+    <t>8cm9q1H5Yx</t>
+  </si>
+  <si>
     <t>7ZxPeHFeIF</t>
   </si>
   <si>
@@ -157,9 +169,15 @@
     <t>S83g9ViAsQ</t>
   </si>
   <si>
+    <t>Kevin Piccola</t>
+  </si>
+  <si>
     <t>Mini Track Head Guy/Starter</t>
   </si>
   <si>
+    <t>Y9RUk8gRqx</t>
+  </si>
+  <si>
     <t>MZMXgMr9pU</t>
   </si>
   <si>
@@ -169,7 +187,7 @@
     <t>9Oa0NXLSYw</t>
   </si>
   <si>
-    <t>jessica swanson</t>
+    <t>Jessica Swanson</t>
   </si>
   <si>
     <t>Mini Track Flagger</t>
@@ -187,19 +205,19 @@
     <t>rlgFbwV61E</t>
   </si>
   <si>
-    <t>Front/Back Gate 7-3</t>
+    <t>Front/Back Gate 7a-3p</t>
   </si>
   <si>
     <t>UJMFPHOX3c</t>
   </si>
   <si>
-    <t>Front/Back Gate 7-9</t>
+    <t>Front/Back Gate 7a-9a</t>
   </si>
   <si>
     <t>9wFrbztqua</t>
   </si>
   <si>
-    <t>Front Gate 7-12</t>
+    <t>Front Gate 7a-12p</t>
   </si>
   <si>
     <t>jqX1P5aAI2</t>
@@ -217,10 +235,10 @@
     <t>H9ws2Dij5N</t>
   </si>
   <si>
-    <t>mark smith</t>
-  </si>
-  <si>
-    <t>Flagger</t>
+    <t>Mark Smith</t>
+  </si>
+  <si>
+    <t>Flagger Sunday</t>
   </si>
   <si>
     <t>lICnUp7PYU</t>
@@ -271,6 +289,60 @@
     <t>xqZcyWX3g2</t>
   </si>
   <si>
+    <t>Flagger Saturday</t>
+  </si>
+  <si>
+    <t>fQpTmpBH7Q</t>
+  </si>
+  <si>
+    <t>uvo8GmIDHm</t>
+  </si>
+  <si>
+    <t>uKgoRmeveK</t>
+  </si>
+  <si>
+    <t>XvZanPOWVh</t>
+  </si>
+  <si>
+    <t>sRssV3IQV7</t>
+  </si>
+  <si>
+    <t>6pxxyAsQHd</t>
+  </si>
+  <si>
+    <t>jukCwhixPa</t>
+  </si>
+  <si>
+    <t>ePfIEyfNkW</t>
+  </si>
+  <si>
+    <t>HQ5896QarP</t>
+  </si>
+  <si>
+    <t>sHFOiUmf3J</t>
+  </si>
+  <si>
+    <t>lfsC79YAAs</t>
+  </si>
+  <si>
+    <t>VQbfjZbKC9</t>
+  </si>
+  <si>
+    <t>3z0Yb6ydQv</t>
+  </si>
+  <si>
+    <t>QVCrAoYG0i</t>
+  </si>
+  <si>
+    <t>2zJSDNIu7T</t>
+  </si>
+  <si>
+    <t>IjVPg7U8He</t>
+  </si>
+  <si>
+    <t>EzNsjXkdfp</t>
+  </si>
+  <si>
     <t>Track Maintenance/Relief Flagger</t>
   </si>
   <si>
@@ -337,7 +409,7 @@
     <t>aIvH8s8Nfe</t>
   </si>
   <si>
-    <t>Sat. Front gate 3-7</t>
+    <t>Sat. Front gate 3p-7p</t>
   </si>
   <si>
     <t>q8LmOBQuHs</t>
@@ -349,7 +421,7 @@
     <t>Adam Swanson</t>
   </si>
   <si>
-    <t>Sat. Front gate 7-11</t>
+    <t>Sat. Front gate 7p-11p</t>
   </si>
   <si>
     <t>DZSkt3OWA0</t>
@@ -370,7 +442,7 @@
     <t>9k3lUOnlXJ</t>
   </si>
   <si>
-    <t>Saturday Signup 7-9</t>
+    <t>Saturday Signup 7p-9p</t>
   </si>
   <si>
     <t>xvUj1j8g3z</t>
@@ -382,6 +454,9 @@
     <t>Saturday Night Watering</t>
   </si>
   <si>
+    <t>xl1U7sUlRl</t>
+  </si>
+  <si>
     <t>PoJOD5hr4c</t>
   </si>
   <si>
@@ -412,7 +487,37 @@
     <t>AzLEzsVkhL</t>
   </si>
   <si>
+    <t>Saturday Morning Signup</t>
+  </si>
+  <si>
+    <t>3ZVfHAWv6H</t>
+  </si>
+  <si>
+    <t>t6m1AQBNfs</t>
+  </si>
+  <si>
+    <t>Saturday Front/Back Gate 7a-3p</t>
+  </si>
+  <si>
+    <t>aOiiBhPJA6</t>
+  </si>
+  <si>
+    <t>Saturday Front/Back Gate 7a-9a</t>
+  </si>
+  <si>
+    <t>5jA2T4zNHi</t>
+  </si>
+  <si>
+    <t>Saturday Front Gate 7a-3p</t>
+  </si>
+  <si>
+    <t>KWuGvXBJPq</t>
+  </si>
+  <si>
     <t>Friday Night Watering</t>
+  </si>
+  <si>
+    <t>iM0dMICTCQ</t>
   </si>
   <si>
     <t>k2zs7OHk1E</t>
@@ -452,7 +557,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="80">
+  <numFmts count="100">
     <numFmt numFmtId="164" formatCode="$0.00"/>
     <numFmt numFmtId="165" formatCode="$0.00"/>
     <numFmt numFmtId="166" formatCode="$0.00"/>
@@ -533,6 +638,26 @@
     <numFmt numFmtId="241" formatCode="$0.00"/>
     <numFmt numFmtId="242" formatCode="$0.00"/>
     <numFmt numFmtId="243" formatCode="$0.00"/>
+    <numFmt numFmtId="244" formatCode="$0.00"/>
+    <numFmt numFmtId="245" formatCode="$0.00"/>
+    <numFmt numFmtId="246" formatCode="$0.00"/>
+    <numFmt numFmtId="247" formatCode="$0.00"/>
+    <numFmt numFmtId="248" formatCode="$0.00"/>
+    <numFmt numFmtId="249" formatCode="$0.00"/>
+    <numFmt numFmtId="250" formatCode="$0.00"/>
+    <numFmt numFmtId="251" formatCode="$0.00"/>
+    <numFmt numFmtId="252" formatCode="$0.00"/>
+    <numFmt numFmtId="253" formatCode="$0.00"/>
+    <numFmt numFmtId="254" formatCode="$0.00"/>
+    <numFmt numFmtId="255" formatCode="$0.00"/>
+    <numFmt numFmtId="256" formatCode="$0.00"/>
+    <numFmt numFmtId="257" formatCode="$0.00"/>
+    <numFmt numFmtId="258" formatCode="$0.00"/>
+    <numFmt numFmtId="259" formatCode="$0.00"/>
+    <numFmt numFmtId="260" formatCode="$0.00"/>
+    <numFmt numFmtId="261" formatCode="$0.00"/>
+    <numFmt numFmtId="262" formatCode="$0.00"/>
+    <numFmt numFmtId="263" formatCode="$0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -587,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -635,7 +760,7 @@
     <xf numFmtId="203" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="204" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="205" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="206" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="206" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="207" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="208" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="209" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -644,15 +769,15 @@
     <xf numFmtId="212" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="213" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="214" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="215" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="216" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="217" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="215" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="216" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="217" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="218" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="219" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="220" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="221" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="221" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="222" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="223" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="223" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="224" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="225" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="226" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -661,18 +786,38 @@
     <xf numFmtId="229" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="230" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="231" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="232" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="233" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="234" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="232" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="233" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="234" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="235" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="236" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="237" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="238" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="238" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="239" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="240" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="241" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="242" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="243" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="244" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="245" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="246" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="247" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="248" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="249" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="250" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="251" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="252" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="253" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="254" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="255" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="256" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="257" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="258" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="259" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="260" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="261" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="262" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="263" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1009,7 +1154,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1265,10 +1410,10 @@
     </row>
     <row r="10" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s" s="3">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3">
         <v>3</v>
@@ -1283,18 +1428,18 @@
         <v>12</v>
       </c>
       <c r="G10" t="s" s="3">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H10" t="s" s="3">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s" s="5">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s" s="5">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5">
         <v>3</v>
@@ -1309,18 +1454,18 @@
         <v>12</v>
       </c>
       <c r="G11" t="s" s="5">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s" s="5">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s" s="3">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C12" s="3">
         <v>3</v>
@@ -1335,10 +1480,10 @@
         <v>12</v>
       </c>
       <c r="G12" t="s" s="3">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s" s="3">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1346,7 +1491,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="5">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C13" s="5">
         <v>3</v>
@@ -1364,7 +1509,7 @@
         <v>12</v>
       </c>
       <c r="H13" t="s" s="5">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1372,7 +1517,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C14" s="3">
         <v>3</v>
@@ -1390,7 +1535,7 @@
         <v>12</v>
       </c>
       <c r="H14" t="s" s="3">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1398,7 +1543,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s" s="18">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C15" s="18">
         <v>1</v>
@@ -1416,15 +1561,15 @@
         <v>12</v>
       </c>
       <c r="H15" t="s" s="18">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s" s="20">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s" s="20">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C16" s="20">
         <v>2</v>
@@ -1439,10 +1584,10 @@
         <v>12</v>
       </c>
       <c r="G16" t="s" s="20">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="H16" t="s" s="20">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1450,7 +1595,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s" s="18">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C17" s="18">
         <v>1.5</v>
@@ -1468,15 +1613,15 @@
         <v>12</v>
       </c>
       <c r="H17" t="s" s="18">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s" s="20">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s" s="20">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C18" s="20">
         <v>1.5</v>
@@ -1491,10 +1636,10 @@
         <v>12</v>
       </c>
       <c r="G18" t="s" s="20">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H18" t="s" s="20">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1502,7 +1647,7 @@
         <v>12</v>
       </c>
       <c r="B19" t="s" s="18">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C19" s="18">
         <v>1.5</v>
@@ -1520,7 +1665,7 @@
         <v>12</v>
       </c>
       <c r="H19" t="s" s="18">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1528,7 +1673,7 @@
         <v>12</v>
       </c>
       <c r="B20" t="s" s="20">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C20" s="20">
         <v>1.5</v>
@@ -1546,7 +1691,7 @@
         <v>12</v>
       </c>
       <c r="H20" t="s" s="20">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1554,7 +1699,7 @@
         <v>12</v>
       </c>
       <c r="B21" t="s" s="5">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C21" s="5">
         <v>3</v>
@@ -1572,7 +1717,7 @@
         <v>12</v>
       </c>
       <c r="H21" t="s" s="5">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1580,7 +1725,7 @@
         <v>12</v>
       </c>
       <c r="B22" t="s" s="20">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C22" s="20">
         <v>1</v>
@@ -1598,7 +1743,7 @@
         <v>12</v>
       </c>
       <c r="H22" t="s" s="20">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1606,7 +1751,7 @@
         <v>12</v>
       </c>
       <c r="B23" t="s" s="5">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C23" s="5">
         <v>1.5</v>
@@ -1624,15 +1769,15 @@
         <v>12</v>
       </c>
       <c r="H23" t="s" s="5">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s" s="3">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s" s="3">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C24" s="3">
         <v>3</v>
@@ -1647,18 +1792,18 @@
         <v>12</v>
       </c>
       <c r="G24" t="s" s="3">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s" s="3">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s" s="18">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s" s="18">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C25" s="18">
         <v>3</v>
@@ -1673,10 +1818,10 @@
         <v>12</v>
       </c>
       <c r="G25" t="s" s="18">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="H25" t="s" s="18">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1684,7 +1829,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s" s="20">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C26" s="20">
         <v>3</v>
@@ -1702,7 +1847,7 @@
         <v>12</v>
       </c>
       <c r="H26" t="s" s="20">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1710,7 +1855,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s" s="18">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C27" s="18">
         <v>3</v>
@@ -1728,7 +1873,7 @@
         <v>12</v>
       </c>
       <c r="H27" t="s" s="18">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1736,7 +1881,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s" s="20">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C28" s="20">
         <v>3</v>
@@ -1754,7 +1899,7 @@
         <v>12</v>
       </c>
       <c r="H28" t="s" s="20">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1762,7 +1907,7 @@
         <v>12</v>
       </c>
       <c r="B29" t="s" s="18">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C29" s="18">
         <v>3</v>
@@ -1780,7 +1925,7 @@
         <v>12</v>
       </c>
       <c r="H29" t="s" s="18">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1788,7 +1933,7 @@
         <v>12</v>
       </c>
       <c r="B30" t="s" s="20">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C30" s="20">
         <v>3</v>
@@ -1806,7 +1951,7 @@
         <v>12</v>
       </c>
       <c r="H30" t="s" s="20">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1814,7 +1959,7 @@
         <v>12</v>
       </c>
       <c r="B31" t="s" s="18">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C31" s="18">
         <v>3</v>
@@ -1832,7 +1977,7 @@
         <v>12</v>
       </c>
       <c r="H31" t="s" s="18">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1840,7 +1985,7 @@
         <v>12</v>
       </c>
       <c r="B32" t="s" s="20">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C32" s="20">
         <v>3</v>
@@ -1858,7 +2003,7 @@
         <v>12</v>
       </c>
       <c r="H32" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1866,7 +2011,7 @@
         <v>12</v>
       </c>
       <c r="B33" t="s" s="18">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C33" s="18">
         <v>3</v>
@@ -1884,7 +2029,7 @@
         <v>12</v>
       </c>
       <c r="H33" t="s" s="18">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1892,7 +2037,7 @@
         <v>12</v>
       </c>
       <c r="B34" t="s" s="20">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C34" s="20">
         <v>3</v>
@@ -1910,7 +2055,7 @@
         <v>12</v>
       </c>
       <c r="H34" t="s" s="20">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1918,7 +2063,7 @@
         <v>12</v>
       </c>
       <c r="B35" t="s" s="18">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C35" s="18">
         <v>3</v>
@@ -1936,7 +2081,7 @@
         <v>12</v>
       </c>
       <c r="H35" t="s" s="18">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1944,7 +2089,7 @@
         <v>12</v>
       </c>
       <c r="B36" t="s" s="20">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C36" s="20">
         <v>3</v>
@@ -1962,7 +2107,7 @@
         <v>12</v>
       </c>
       <c r="H36" t="s" s="20">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1970,7 +2115,7 @@
         <v>12</v>
       </c>
       <c r="B37" t="s" s="18">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C37" s="18">
         <v>3</v>
@@ -1988,7 +2133,7 @@
         <v>12</v>
       </c>
       <c r="H37" t="s" s="18">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1996,7 +2141,7 @@
         <v>12</v>
       </c>
       <c r="B38" t="s" s="20">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C38" s="20">
         <v>3</v>
@@ -2014,7 +2159,7 @@
         <v>12</v>
       </c>
       <c r="H38" t="s" s="20">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2022,7 +2167,7 @@
         <v>12</v>
       </c>
       <c r="B39" t="s" s="18">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C39" s="18">
         <v>3</v>
@@ -2040,7 +2185,7 @@
         <v>12</v>
       </c>
       <c r="H39" t="s" s="18">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2048,13 +2193,13 @@
         <v>12</v>
       </c>
       <c r="B40" t="s" s="20">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C40" s="20">
         <v>3</v>
       </c>
       <c r="D40" s="45">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E40" t="s" s="20">
         <v>11</v>
@@ -2066,7 +2211,7 @@
         <v>12</v>
       </c>
       <c r="H40" t="s" s="20">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2074,13 +2219,13 @@
         <v>12</v>
       </c>
       <c r="B41" t="s" s="18">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C41" s="18">
         <v>3</v>
       </c>
       <c r="D41" s="46">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E41" t="s" s="18">
         <v>11</v>
@@ -2092,33 +2237,33 @@
         <v>12</v>
       </c>
       <c r="H41" t="s" s="18">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="B42" t="s" s="3">
-        <v>85</v>
-      </c>
-      <c r="C42" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B42" t="s" s="20">
+        <v>91</v>
+      </c>
+      <c r="C42" s="20">
         <v>3</v>
       </c>
       <c r="D42" s="47">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="F42" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="G42" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="H42" t="s" s="3">
-        <v>88</v>
+        <v>75</v>
+      </c>
+      <c r="E42" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H42" t="s" s="20">
+        <v>94</v>
       </c>
     </row>
     <row r="43" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2126,13 +2271,13 @@
         <v>12</v>
       </c>
       <c r="B43" t="s" s="18">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C43" s="18">
         <v>3</v>
       </c>
       <c r="D43" s="48">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E43" t="s" s="18">
         <v>11</v>
@@ -2144,7 +2289,7 @@
         <v>12</v>
       </c>
       <c r="H43" t="s" s="18">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2152,13 +2297,13 @@
         <v>12</v>
       </c>
       <c r="B44" t="s" s="20">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C44" s="20">
         <v>3</v>
       </c>
       <c r="D44" s="49">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E44" t="s" s="20">
         <v>11</v>
@@ -2170,7 +2315,7 @@
         <v>12</v>
       </c>
       <c r="H44" t="s" s="20">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2178,13 +2323,13 @@
         <v>12</v>
       </c>
       <c r="B45" t="s" s="18">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C45" s="18">
         <v>3</v>
       </c>
       <c r="D45" s="50">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E45" t="s" s="18">
         <v>11</v>
@@ -2196,7 +2341,7 @@
         <v>12</v>
       </c>
       <c r="H45" t="s" s="18">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2204,13 +2349,13 @@
         <v>12</v>
       </c>
       <c r="B46" t="s" s="20">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D46" s="51">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E46" t="s" s="20">
         <v>11</v>
@@ -2222,7 +2367,7 @@
         <v>12</v>
       </c>
       <c r="H46" t="s" s="20">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2230,13 +2375,13 @@
         <v>12</v>
       </c>
       <c r="B47" t="s" s="18">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C47" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D47" s="52">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E47" t="s" s="18">
         <v>11</v>
@@ -2248,7 +2393,7 @@
         <v>12</v>
       </c>
       <c r="H47" t="s" s="18">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2256,13 +2401,13 @@
         <v>12</v>
       </c>
       <c r="B48" t="s" s="20">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C48" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D48" s="53">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E48" t="s" s="20">
         <v>11</v>
@@ -2274,7 +2419,7 @@
         <v>12</v>
       </c>
       <c r="H48" t="s" s="20">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2282,13 +2427,13 @@
         <v>12</v>
       </c>
       <c r="B49" t="s" s="18">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C49" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D49" s="54">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E49" t="s" s="18">
         <v>11</v>
@@ -2300,7 +2445,7 @@
         <v>12</v>
       </c>
       <c r="H49" t="s" s="18">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2308,13 +2453,13 @@
         <v>12</v>
       </c>
       <c r="B50" t="s" s="20">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C50" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" s="55">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E50" t="s" s="20">
         <v>11</v>
@@ -2326,85 +2471,85 @@
         <v>12</v>
       </c>
       <c r="H50" t="s" s="20">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s" s="5">
-        <v>99</v>
-      </c>
-      <c r="B51" t="s" s="5">
-        <v>100</v>
-      </c>
-      <c r="C51" s="5">
-        <v>0</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B51" t="s" s="18">
+        <v>91</v>
+      </c>
+      <c r="C51" s="18">
+        <v>3</v>
       </c>
       <c r="D51" s="56">
-        <v>600</v>
-      </c>
-      <c r="E51" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F51" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="G51" t="s" s="5">
-        <v>101</v>
-      </c>
-      <c r="H51" t="s" s="5">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="52" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="B52" t="s" s="3">
+        <v>75</v>
+      </c>
+      <c r="E51" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G51" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H51" t="s" s="18">
         <v>103</v>
       </c>
-      <c r="C52" s="3">
+    </row>
+    <row r="52" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B52" t="s" s="20">
+        <v>91</v>
+      </c>
+      <c r="C52" s="20">
         <v>3</v>
       </c>
       <c r="D52" s="57">
-        <v>125</v>
-      </c>
-      <c r="E52" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="F52" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="G52" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="H52" t="s" s="3">
+        <v>75</v>
+      </c>
+      <c r="E52" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F52" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G52" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H52" t="s" s="20">
         <v>104</v>
       </c>
     </row>
-    <row r="53" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="B53" t="s" s="5">
-        <v>105</v>
-      </c>
-      <c r="C53" s="5">
+    <row r="53" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B53" t="s" s="18">
+        <v>91</v>
+      </c>
+      <c r="C53" s="18">
         <v>3</v>
       </c>
       <c r="D53" s="58">
         <v>75</v>
       </c>
-      <c r="E53" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F53" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="G53" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="H53" t="s" s="5">
-        <v>106</v>
+      <c r="E53" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H53" t="s" s="18">
+        <v>105</v>
       </c>
     </row>
     <row r="54" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2412,13 +2557,13 @@
         <v>12</v>
       </c>
       <c r="B54" t="s" s="20">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C54" s="20">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="D54" s="59">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E54" t="s" s="20">
         <v>11</v>
@@ -2430,7 +2575,7 @@
         <v>12</v>
       </c>
       <c r="H54" t="s" s="20">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2438,77 +2583,77 @@
         <v>12</v>
       </c>
       <c r="B55" t="s" s="18">
+        <v>91</v>
+      </c>
+      <c r="C55" s="18">
+        <v>3</v>
+      </c>
+      <c r="D55" s="60">
+        <v>75</v>
+      </c>
+      <c r="E55" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F55" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G55" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H55" t="s" s="18">
         <v>107</v>
-      </c>
-      <c r="C55" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="D55" s="60">
-        <v>0</v>
-      </c>
-      <c r="E55" t="s" s="18">
-        <v>11</v>
-      </c>
-      <c r="F55" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="G55" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="H55" t="s" s="18">
-        <v>109</v>
       </c>
     </row>
     <row r="56" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B56" t="s" s="20">
+        <v>91</v>
+      </c>
+      <c r="C56" s="20">
+        <v>3</v>
+      </c>
+      <c r="D56" s="61">
+        <v>75</v>
+      </c>
+      <c r="E56" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F56" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G56" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H56" t="s" s="20">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B57" t="s" s="18">
+        <v>109</v>
+      </c>
+      <c r="C57" s="18">
+        <v>3</v>
+      </c>
+      <c r="D57" s="62">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F57" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G57" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H57" t="s" s="18">
         <v>110</v>
-      </c>
-      <c r="B56" t="s" s="20">
-        <v>111</v>
-      </c>
-      <c r="C56" s="20">
-        <v>1.5</v>
-      </c>
-      <c r="D56" s="61">
-        <v>0</v>
-      </c>
-      <c r="E56" t="s" s="20">
-        <v>11</v>
-      </c>
-      <c r="F56" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="G56" t="s" s="20">
-        <v>112</v>
-      </c>
-      <c r="H56" t="s" s="20">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="57" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s" s="5">
-        <v>114</v>
-      </c>
-      <c r="B57" t="s" s="5">
-        <v>115</v>
-      </c>
-      <c r="C57" s="5">
-        <v>0</v>
-      </c>
-      <c r="D57" s="62">
-        <v>40</v>
-      </c>
-      <c r="E57" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F57" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="G57" t="s" s="5">
-        <v>116</v>
-      </c>
-      <c r="H57" t="s" s="5">
-        <v>117</v>
       </c>
     </row>
     <row r="58" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2516,10 +2661,10 @@
         <v>12</v>
       </c>
       <c r="B58" t="s" s="20">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C58" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D58" s="63">
         <v>0</v>
@@ -2534,33 +2679,33 @@
         <v>12</v>
       </c>
       <c r="H58" t="s" s="20">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="59" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="B59" t="s" s="18">
-        <v>118</v>
-      </c>
-      <c r="C59" s="18">
-        <v>1</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="B59" t="s" s="5">
+        <v>109</v>
+      </c>
+      <c r="C59" s="5">
+        <v>3</v>
       </c>
       <c r="D59" s="64">
         <v>0</v>
       </c>
-      <c r="E59" t="s" s="18">
-        <v>11</v>
-      </c>
-      <c r="F59" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="G59" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="H59" t="s" s="18">
-        <v>120</v>
+      <c r="E59" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F59" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="H59" t="s" s="5">
+        <v>112</v>
       </c>
     </row>
     <row r="60" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2568,10 +2713,10 @@
         <v>12</v>
       </c>
       <c r="B60" t="s" s="20">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C60" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D60" s="65">
         <v>0</v>
@@ -2586,7 +2731,7 @@
         <v>12</v>
       </c>
       <c r="H60" t="s" s="20">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2594,10 +2739,10 @@
         <v>12</v>
       </c>
       <c r="B61" t="s" s="18">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C61" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D61" s="66">
         <v>0</v>
@@ -2612,7 +2757,7 @@
         <v>12</v>
       </c>
       <c r="H61" t="s" s="18">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2620,10 +2765,10 @@
         <v>12</v>
       </c>
       <c r="B62" t="s" s="20">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C62" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D62" s="67">
         <v>0</v>
@@ -2638,7 +2783,7 @@
         <v>12</v>
       </c>
       <c r="H62" t="s" s="20">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2646,10 +2791,10 @@
         <v>12</v>
       </c>
       <c r="B63" t="s" s="18">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C63" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D63" s="68">
         <v>0</v>
@@ -2664,7 +2809,7 @@
         <v>12</v>
       </c>
       <c r="H63" t="s" s="18">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2672,10 +2817,10 @@
         <v>12</v>
       </c>
       <c r="B64" t="s" s="20">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C64" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64" s="69">
         <v>0</v>
@@ -2690,7 +2835,7 @@
         <v>12</v>
       </c>
       <c r="H64" t="s" s="20">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2698,10 +2843,10 @@
         <v>12</v>
       </c>
       <c r="B65" t="s" s="18">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C65" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65" s="70">
         <v>0</v>
@@ -2716,7 +2861,7 @@
         <v>12</v>
       </c>
       <c r="H65" t="s" s="18">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2724,10 +2869,10 @@
         <v>12</v>
       </c>
       <c r="B66" t="s" s="20">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C66" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66" s="71">
         <v>0</v>
@@ -2742,7 +2887,7 @@
         <v>12</v>
       </c>
       <c r="H66" t="s" s="20">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2768,85 +2913,85 @@
         <v>12</v>
       </c>
       <c r="H67" t="s" s="18">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s" s="3">
+        <v>123</v>
+      </c>
+      <c r="B68" t="s" s="3">
+        <v>124</v>
+      </c>
+      <c r="C68" s="3">
+        <v>0</v>
+      </c>
+      <c r="D68" s="73">
+        <v>600</v>
+      </c>
+      <c r="E68" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="F68" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="G68" t="s" s="3">
+        <v>125</v>
+      </c>
+      <c r="H68" t="s" s="3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="B69" t="s" s="5">
+        <v>127</v>
+      </c>
+      <c r="C69" s="5">
+        <v>3</v>
+      </c>
+      <c r="D69" s="74">
+        <v>125</v>
+      </c>
+      <c r="E69" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="G69" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="H69" t="s" s="5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="B70" t="s" s="3">
         <v>129</v>
       </c>
-    </row>
-    <row r="68" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="B68" t="s" s="20">
-        <v>121</v>
-      </c>
-      <c r="C68" s="20">
-        <v>2</v>
-      </c>
-      <c r="D68" s="73">
-        <v>0</v>
-      </c>
-      <c r="E68" t="s" s="20">
-        <v>11</v>
-      </c>
-      <c r="F68" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="G68" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="H68" t="s" s="20">
+      <c r="C70" s="3">
+        <v>3</v>
+      </c>
+      <c r="D70" s="75">
+        <v>75</v>
+      </c>
+      <c r="E70" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="F70" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="H70" t="s" s="3">
         <v>130</v>
-      </c>
-    </row>
-    <row r="69" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="B69" t="s" s="18">
-        <v>121</v>
-      </c>
-      <c r="C69" s="18">
-        <v>2</v>
-      </c>
-      <c r="D69" s="74">
-        <v>0</v>
-      </c>
-      <c r="E69" t="s" s="18">
-        <v>11</v>
-      </c>
-      <c r="F69" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="G69" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="H69" t="s" s="18">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="70" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="B70" t="s" s="20">
-        <v>132</v>
-      </c>
-      <c r="C70" s="20">
-        <v>2</v>
-      </c>
-      <c r="D70" s="75">
-        <v>0</v>
-      </c>
-      <c r="E70" t="s" s="20">
-        <v>11</v>
-      </c>
-      <c r="F70" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="G70" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="H70" t="s" s="20">
-        <v>133</v>
       </c>
     </row>
     <row r="71" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2854,25 +2999,25 @@
         <v>12</v>
       </c>
       <c r="B71" t="s" s="18">
+        <v>131</v>
+      </c>
+      <c r="C71" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="D71" s="76">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F71" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G71" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H71" t="s" s="18">
         <v>132</v>
-      </c>
-      <c r="C71" s="18">
-        <v>2</v>
-      </c>
-      <c r="D71" s="76">
-        <v>0</v>
-      </c>
-      <c r="E71" t="s" s="18">
-        <v>11</v>
-      </c>
-      <c r="F71" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="G71" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="H71" t="s" s="18">
-        <v>134</v>
       </c>
     </row>
     <row r="72" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2880,10 +3025,10 @@
         <v>12</v>
       </c>
       <c r="B72" t="s" s="20">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C72" s="20">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D72" s="77">
         <v>0</v>
@@ -2898,18 +3043,18 @@
         <v>12</v>
       </c>
       <c r="H72" t="s" s="20">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="73" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s" s="18">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="B73" t="s" s="18">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C73" s="18">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D73" s="78">
         <v>0</v>
@@ -2921,36 +3066,36 @@
         <v>12</v>
       </c>
       <c r="G73" t="s" s="18">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="H73" t="s" s="18">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="74" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="B74" t="s" s="20">
-        <v>132</v>
-      </c>
-      <c r="C74" s="20">
-        <v>2</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s" s="3">
+        <v>138</v>
+      </c>
+      <c r="B74" t="s" s="3">
+        <v>139</v>
+      </c>
+      <c r="C74" s="3">
+        <v>0</v>
       </c>
       <c r="D74" s="79">
-        <v>0</v>
-      </c>
-      <c r="E74" t="s" s="20">
-        <v>11</v>
-      </c>
-      <c r="F74" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="G74" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="H74" t="s" s="20">
-        <v>137</v>
+        <v>40</v>
+      </c>
+      <c r="E74" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="F74" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="G74" t="s" s="3">
+        <v>140</v>
+      </c>
+      <c r="H74" t="s" s="3">
+        <v>141</v>
       </c>
     </row>
     <row r="75" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2958,10 +3103,10 @@
         <v>12</v>
       </c>
       <c r="B75" t="s" s="18">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C75" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D75" s="80">
         <v>0</v>
@@ -2976,7 +3121,7 @@
         <v>12</v>
       </c>
       <c r="H75" t="s" s="18">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2984,10 +3129,10 @@
         <v>12</v>
       </c>
       <c r="B76" t="s" s="20">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C76" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D76" s="81">
         <v>0</v>
@@ -3002,15 +3147,15 @@
         <v>12</v>
       </c>
       <c r="H76" t="s" s="20">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s" s="18">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B77" t="s" s="18">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C77" s="18">
         <v>2</v>
@@ -3025,10 +3170,10 @@
         <v>12</v>
       </c>
       <c r="G77" t="s" s="18">
-        <v>12</v>
+        <v>146</v>
       </c>
       <c r="H77" t="s" s="18">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -3036,7 +3181,7 @@
         <v>12</v>
       </c>
       <c r="B78" t="s" s="20">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C78" s="20">
         <v>2</v>
@@ -3054,7 +3199,7 @@
         <v>12</v>
       </c>
       <c r="H78" t="s" s="20">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -3062,7 +3207,7 @@
         <v>12</v>
       </c>
       <c r="B79" t="s" s="18">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C79" s="18">
         <v>2</v>
@@ -3080,12 +3225,572 @@
         <v>12</v>
       </c>
       <c r="H79" t="s" s="18">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>143</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B80" t="s" s="20">
+        <v>145</v>
+      </c>
+      <c r="C80" s="20">
+        <v>2</v>
+      </c>
+      <c r="D80" s="85">
+        <v>0</v>
+      </c>
+      <c r="E80" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F80" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G80" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H80" t="s" s="20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B81" t="s" s="18">
+        <v>145</v>
+      </c>
+      <c r="C81" s="18">
+        <v>2</v>
+      </c>
+      <c r="D81" s="86">
+        <v>0</v>
+      </c>
+      <c r="E81" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F81" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H81" t="s" s="18">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="82" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B82" t="s" s="20">
+        <v>145</v>
+      </c>
+      <c r="C82" s="20">
+        <v>2</v>
+      </c>
+      <c r="D82" s="87">
+        <v>0</v>
+      </c>
+      <c r="E82" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F82" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G82" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H82" t="s" s="20">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B83" t="s" s="18">
+        <v>145</v>
+      </c>
+      <c r="C83" s="18">
+        <v>2</v>
+      </c>
+      <c r="D83" s="88">
+        <v>0</v>
+      </c>
+      <c r="E83" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F83" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G83" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H83" t="s" s="18">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="84" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B84" t="s" s="20">
+        <v>145</v>
+      </c>
+      <c r="C84" s="20">
+        <v>2</v>
+      </c>
+      <c r="D84" s="89">
+        <v>0</v>
+      </c>
+      <c r="E84" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F84" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G84" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H84" t="s" s="20">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="85" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B85" t="s" s="18">
+        <v>145</v>
+      </c>
+      <c r="C85" s="18">
+        <v>2</v>
+      </c>
+      <c r="D85" s="90">
+        <v>0</v>
+      </c>
+      <c r="E85" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F85" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G85" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H85" t="s" s="18">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B86" t="s" s="20">
+        <v>145</v>
+      </c>
+      <c r="C86" s="20">
+        <v>2</v>
+      </c>
+      <c r="D86" s="91">
+        <v>0</v>
+      </c>
+      <c r="E86" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F86" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G86" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H86" t="s" s="20">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="87" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B87" t="s" s="18">
+        <v>157</v>
+      </c>
+      <c r="E87" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F87" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G87" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H87" t="s" s="18">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="88" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B88" t="s" s="20">
+        <v>157</v>
+      </c>
+      <c r="E88" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F88" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G88" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H88" t="s" s="20">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="89" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B89" t="s" s="18">
+        <v>160</v>
+      </c>
+      <c r="C89" s="18">
+        <v>3</v>
+      </c>
+      <c r="D89" s="92">
+        <v>75</v>
+      </c>
+      <c r="E89" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F89" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G89" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H89" t="s" s="18">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="90" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B90" t="s" s="20">
+        <v>162</v>
+      </c>
+      <c r="C90" s="20">
+        <v>1</v>
+      </c>
+      <c r="D90" s="93">
+        <v>25</v>
+      </c>
+      <c r="E90" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F90" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G90" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H90" t="s" s="20">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="91" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B91" t="s" s="18">
+        <v>164</v>
+      </c>
+      <c r="C91" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="D91" s="94">
+        <v>50</v>
+      </c>
+      <c r="E91" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F91" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G91" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H91" t="s" s="18">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s" s="20">
+        <v>51</v>
+      </c>
+      <c r="B92" t="s" s="20">
+        <v>166</v>
+      </c>
+      <c r="C92" s="20">
+        <v>2</v>
+      </c>
+      <c r="D92" s="95">
+        <v>0</v>
+      </c>
+      <c r="E92" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F92" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G92" t="s" s="20">
+        <v>167</v>
+      </c>
+      <c r="H92" t="s" s="20">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="93" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B93" t="s" s="18">
+        <v>166</v>
+      </c>
+      <c r="C93" s="18">
+        <v>2</v>
+      </c>
+      <c r="D93" s="96">
+        <v>0</v>
+      </c>
+      <c r="E93" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F93" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G93" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H93" t="s" s="18">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="94" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B94" t="s" s="20">
+        <v>166</v>
+      </c>
+      <c r="C94" s="20">
+        <v>2</v>
+      </c>
+      <c r="D94" s="97">
+        <v>0</v>
+      </c>
+      <c r="E94" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F94" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G94" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H94" t="s" s="20">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B95" t="s" s="18">
+        <v>166</v>
+      </c>
+      <c r="C95" s="18">
+        <v>2</v>
+      </c>
+      <c r="D95" s="98">
+        <v>0</v>
+      </c>
+      <c r="E95" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F95" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G95" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H95" t="s" s="18">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="96" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B96" t="s" s="20">
+        <v>166</v>
+      </c>
+      <c r="C96" s="20">
+        <v>2</v>
+      </c>
+      <c r="D96" s="99">
+        <v>0</v>
+      </c>
+      <c r="E96" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F96" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G96" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H96" t="s" s="20">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="97" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B97" t="s" s="18">
+        <v>166</v>
+      </c>
+      <c r="C97" s="18">
+        <v>2</v>
+      </c>
+      <c r="D97" s="100">
+        <v>0</v>
+      </c>
+      <c r="E97" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F97" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G97" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H97" t="s" s="18">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="98" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B98" t="s" s="20">
+        <v>166</v>
+      </c>
+      <c r="C98" s="20">
+        <v>2</v>
+      </c>
+      <c r="D98" s="101">
+        <v>0</v>
+      </c>
+      <c r="E98" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F98" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G98" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H98" t="s" s="20">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="99" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B99" t="s" s="18">
+        <v>166</v>
+      </c>
+      <c r="C99" s="18">
+        <v>2</v>
+      </c>
+      <c r="D99" s="102">
+        <v>0</v>
+      </c>
+      <c r="E99" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F99" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G99" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H99" t="s" s="18">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="100" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B100" t="s" s="20">
+        <v>166</v>
+      </c>
+      <c r="C100" s="20">
+        <v>2</v>
+      </c>
+      <c r="D100" s="103">
+        <v>0</v>
+      </c>
+      <c r="E100" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="F100" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="G100" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="H100" t="s" s="20">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="101" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B101" t="s" s="18">
+        <v>166</v>
+      </c>
+      <c r="C101" s="18">
+        <v>2</v>
+      </c>
+      <c r="D101" s="104">
+        <v>0</v>
+      </c>
+      <c r="E101" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="F101" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="G101" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="H101" t="s" s="18">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>